<commit_message>
change file dir and start data vis
</commit_message>
<xml_diff>
--- a/data/36_4_7.xlsx
+++ b/data/36_4_7.xlsx
@@ -73,7 +73,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,6 +85,12 @@
       <sz val="12"/>
       <color rgb="FF3366ff"/>
       <name val="宋体"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -350,13 +356,13 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -891,7 +897,7 @@
     <col min="30" max="30" style="13" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="30">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="14" t="s">
@@ -937,7 +943,7 @@
       <c r="AC1" s="21"/>
       <c r="AD1" s="22"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
@@ -1029,7 +1035,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1037,7 +1043,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="44">
-        <v>2.4285185185185187</v>
+        <v>2.428518518518519</v>
       </c>
       <c r="D3" s="45">
         <v>1.185</v>
@@ -1121,7 +1127,7 @@
         <v>5.809682804674469</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -1213,7 +1219,7 @@
         <v>6.960784313725485</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1305,7 +1311,7 @@
         <v>7.514910536779339</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1397,7 +1403,7 @@
         <v>9.066213921901534</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -1489,7 +1495,7 @@
         <v>7.266775777414081</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1581,7 +1587,7 @@
         <v>6.396694214876021</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1673,7 +1679,7 @@
         <v>6.233009708737858</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -1765,7 +1771,7 @@
         <v>5.374771480804394</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -1857,7 +1863,7 @@
         <v>8.92045454545454</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
@@ -1949,7 +1955,7 @@
         <v>8.031914893617033</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
@@ -2041,7 +2047,7 @@
         <v>7.292817679558005</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
@@ -2133,7 +2139,7 @@
         <v>5.459459459459472</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="1" t="s">
         <v>8</v>
       </c>
@@ -2225,7 +2231,7 @@
         <v>3.5869565217391117</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
@@ -2317,7 +2323,7 @@
         <v>6.063268892794376</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="1" t="s">
         <v>7</v>
       </c>
@@ -2409,7 +2415,7 @@
         <v>11.896551724137954</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="1" t="s">
         <v>7</v>
       </c>
@@ -2501,7 +2507,7 @@
         <v>6.457627118644062</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
@@ -2593,7 +2599,7 @@
         <v>9.95348837209304</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="1" t="s">
         <v>6</v>
       </c>
@@ -2685,7 +2691,7 @@
         <v>6.500888099467135</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="1" t="s">
         <v>7</v>
       </c>
@@ -2777,7 +2783,7 @@
         <v>4.585365853658553</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="1" t="s">
         <v>7</v>
       </c>
@@ -2869,7 +2875,7 @@
         <v>6.3942307692307745</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="1" t="s">
         <v>7</v>
       </c>
@@ -2961,7 +2967,7 @@
         <v>6.442953020134234</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="1" t="s">
         <v>7</v>
       </c>
@@ -3053,7 +3059,7 @@
         <v>6.828358208955217</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="1" t="s">
         <v>7</v>
       </c>
@@ -3145,7 +3151,7 @@
         <v>7.830508474576259</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="1" t="s">
         <v>8</v>
       </c>

</xml_diff>